<commit_message>
adding loopflopy installation instructions and example 3
</commit_message>
<xml_diff>
--- a/examples/Example 3 - Heterogeneity/data/example_data.xlsx
+++ b/examples/Example 3 - Heterogeneity/data/example_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00105295\Projects\loopflopy\examples\Example 3 - Heterogeneity\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BF916EF-E708-41BB-8292-7F869A59D0F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08979D37-405E-4DBC-8C0B-A6E8ABF1195F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="18430" windowHeight="11020" tabRatio="1000" activeTab="4" xr2:uid="{BEB68924-1CF9-4A8C-BED3-3B7C03CCF6FB}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" tabRatio="1000" activeTab="4" xr2:uid="{BEB68924-1CF9-4A8C-BED3-3B7C03CCF6FB}"/>
   </bookViews>
   <sheets>
     <sheet name="strat" sheetId="22" r:id="rId1"/>
@@ -1594,8 +1594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66F73DEA-878D-4205-88DA-BE6F7A54869E}">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1737,7 +1737,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="26">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F7" s="27"/>
       <c r="G7" s="26"/>
@@ -1757,7 +1757,7 @@
         <v>2</v>
       </c>
       <c r="E8" s="26">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F8" s="27"/>
       <c r="G8" s="26"/>
@@ -1777,7 +1777,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="26">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F9" s="27"/>
       <c r="G9" s="26"/>
@@ -1797,7 +1797,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="26">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F10" s="27"/>
       <c r="G10" s="26"/>
@@ -2054,7 +2054,7 @@
         <v>4</v>
       </c>
       <c r="E24" s="26">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="13" x14ac:dyDescent="0.25">
@@ -2088,7 +2088,7 @@
         <v>4</v>
       </c>
       <c r="E26" s="26">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="13" x14ac:dyDescent="0.25">
@@ -2105,7 +2105,7 @@
         <v>4</v>
       </c>
       <c r="E27" s="26">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="13" x14ac:dyDescent="0.25">
@@ -2360,7 +2360,7 @@
         <v>6</v>
       </c>
       <c r="E42" s="26">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
processed observation points using pandas
</commit_message>
<xml_diff>
--- a/examples/Example 3 - Heterogeneity/data/example_data.xlsx
+++ b/examples/Example 3 - Heterogeneity/data/example_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00105295\Projects\loopflopy\examples\Example 3 - Heterogeneity\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08979D37-405E-4DBC-8C0B-A6E8ABF1195F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070846C1-2E68-4A49-A5D7-CEBD8AB5ECE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" tabRatio="1000" activeTab="4" xr2:uid="{BEB68924-1CF9-4A8C-BED3-3B7C03CCF6FB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="18430" windowHeight="11020" tabRatio="1000" activeTab="3" xr2:uid="{BEB68924-1CF9-4A8C-BED3-3B7C03CCF6FB}"/>
   </bookViews>
   <sheets>
     <sheet name="strat" sheetId="22" r:id="rId1"/>
@@ -1419,7 +1419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9173966-0664-454B-A7FA-7F2B0A9E9269}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -1594,7 +1594,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66F73DEA-878D-4205-88DA-BE6F7A54869E}">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updating properties objects for plotting
</commit_message>
<xml_diff>
--- a/examples/Example 3 - Heterogeneity/data/example_data.xlsx
+++ b/examples/Example 3 - Heterogeneity/data/example_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00105295\Projects\loopflopy\examples\Example 3 - Heterogeneity\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070846C1-2E68-4A49-A5D7-CEBD8AB5ECE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{161F3D9B-A051-4D95-AE97-002891232A7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="18430" windowHeight="11020" tabRatio="1000" activeTab="3" xr2:uid="{BEB68924-1CF9-4A8C-BED3-3B7C03CCF6FB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="18430" windowHeight="11020" tabRatio="1000" activeTab="6" xr2:uid="{BEB68924-1CF9-4A8C-BED3-3B7C03CCF6FB}"/>
   </bookViews>
   <sheets>
     <sheet name="strat" sheetId="22" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="obs_bores" sheetId="23" r:id="rId4"/>
     <sheet name="pilot_points" sheetId="27" r:id="rId5"/>
     <sheet name="pumping_bores" sheetId="24" r:id="rId6"/>
+    <sheet name="truth" sheetId="28" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">geo_bores!#REF!</definedName>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="102">
   <si>
     <t>Easting</t>
   </si>
@@ -313,13 +314,49 @@
   </si>
   <si>
     <t>PP45</t>
+  </si>
+  <si>
+    <t>mean_kv</t>
+  </si>
+  <si>
+    <t>mean_ss</t>
+  </si>
+  <si>
+    <t>mean_sy</t>
+  </si>
+  <si>
+    <t>min_kh</t>
+  </si>
+  <si>
+    <t>max_kh</t>
+  </si>
+  <si>
+    <t>min_kv</t>
+  </si>
+  <si>
+    <t>max_kv</t>
+  </si>
+  <si>
+    <t>min_sy</t>
+  </si>
+  <si>
+    <t>max_sy</t>
+  </si>
+  <si>
+    <t>min_ss</t>
+  </si>
+  <si>
+    <t>max_ss</t>
+  </si>
+  <si>
+    <t>kv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -360,8 +397,32 @@
       <sz val="8"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -371,6 +432,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9999"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -387,7 +478,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -459,13 +550,103 @@
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -474,6 +655,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF9999"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1170,7 +1356,7 @@
       <selection activeCell="E15" sqref="E15"/>
       <selection pane="topRight" activeCell="E15" sqref="E15"/>
       <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
-      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomRight" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.25"/>
@@ -1419,8 +1605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9173966-0664-454B-A7FA-7F2B0A9E9269}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection sqref="A1:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1592,843 +1778,2421 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66F73DEA-878D-4205-88DA-BE6F7A54869E}">
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="8.7265625" style="25"/>
-    <col min="5" max="6" width="11.08984375" style="25" customWidth="1"/>
-    <col min="7" max="7" width="8.7265625" style="25"/>
+    <col min="1" max="1" width="4.1796875" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.90625" style="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.90625" style="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.54296875" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.453125" style="26" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.36328125" style="26" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.453125" style="26" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.08984375" style="26" customWidth="1"/>
+    <col min="9" max="9" width="5.81640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.36328125" style="25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.90625" style="25" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.36328125" style="25" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.90625" style="25" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.453125" style="25" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.36328125" style="25" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.453125" style="25" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.7265625" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A1" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="29" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="10"/>
-    </row>
-    <row r="2" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="F1" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="I1" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="J1" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="K1" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="L1" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="M1" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="N1" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="O1" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="P1" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A2" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="31">
         <v>380000</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="31">
         <v>6535000</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="30" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="26">
         <v>10</v>
       </c>
-      <c r="F2" s="27"/>
-      <c r="G2" s="26"/>
-      <c r="I2" s="10"/>
-    </row>
-    <row r="3" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="F2" s="27">
+        <v>1</v>
+      </c>
+      <c r="G2" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H2" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I2" s="25">
+        <v>1</v>
+      </c>
+      <c r="J2" s="25">
+        <v>100</v>
+      </c>
+      <c r="K2" s="25">
+        <f>I2/10</f>
+        <v>0.1</v>
+      </c>
+      <c r="L2" s="25">
+        <f>J2/10</f>
+        <v>10</v>
+      </c>
+      <c r="M2" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="N2" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="O2" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P2" s="25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A3" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="31">
         <v>360000</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="31">
         <v>6537000</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="30" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="26">
         <v>5</v>
       </c>
-      <c r="F3" s="27"/>
-      <c r="G3" s="26"/>
-      <c r="I3" s="10"/>
-    </row>
-    <row r="4" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+      <c r="F3" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="G3" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H3" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I3" s="25">
+        <v>1</v>
+      </c>
+      <c r="J3" s="25">
+        <v>100</v>
+      </c>
+      <c r="K3" s="25">
+        <f t="shared" ref="K3:K46" si="0">I3/10</f>
+        <v>0.1</v>
+      </c>
+      <c r="L3" s="25">
+        <f t="shared" ref="L3:L46" si="1">J3/10</f>
+        <v>10</v>
+      </c>
+      <c r="M3" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="N3" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="O3" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P3" s="25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A4" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="31">
         <v>370000</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="31">
         <v>6530000</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="30" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="26">
         <v>10</v>
       </c>
-      <c r="F4" s="27"/>
-      <c r="G4" s="26"/>
-      <c r="I4" s="10"/>
-    </row>
-    <row r="5" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+      <c r="F4" s="27">
+        <v>1</v>
+      </c>
+      <c r="G4" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H4" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I4" s="25">
+        <v>1</v>
+      </c>
+      <c r="J4" s="25">
+        <v>100</v>
+      </c>
+      <c r="K4" s="25">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="L4" s="25">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="M4" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="N4" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="O4" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P4" s="25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A5" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="31">
         <v>375000</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="31">
         <v>6520000</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="30" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="26">
         <v>100</v>
       </c>
-      <c r="F5" s="27"/>
-      <c r="G5" s="26"/>
-      <c r="I5" s="10"/>
-    </row>
-    <row r="6" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+      <c r="F5" s="27">
+        <v>10</v>
+      </c>
+      <c r="G5" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H5" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I5" s="25">
+        <v>1</v>
+      </c>
+      <c r="J5" s="25">
+        <v>100</v>
+      </c>
+      <c r="K5" s="25">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="L5" s="25">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="M5" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="N5" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="O5" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P5" s="25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A6" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="31">
         <v>385000</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="31">
         <v>6515000</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="30" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="26">
         <v>10</v>
       </c>
-      <c r="F6" s="27"/>
-      <c r="G6" s="26"/>
-      <c r="I6" s="10"/>
-    </row>
-    <row r="7" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+      <c r="F6" s="27">
+        <v>1</v>
+      </c>
+      <c r="G6" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H6" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I6" s="25">
+        <v>1</v>
+      </c>
+      <c r="J6" s="25">
+        <v>100</v>
+      </c>
+      <c r="K6" s="25">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="L6" s="25">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="M6" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="N6" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="O6" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P6" s="25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A7" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="31">
         <v>375000</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="31">
         <v>6540000</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="30" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="26">
         <v>2</v>
       </c>
-      <c r="F7" s="27"/>
-      <c r="G7" s="26"/>
-      <c r="I7" s="10"/>
-    </row>
-    <row r="8" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+      <c r="F7" s="27">
+        <v>0.2</v>
+      </c>
+      <c r="G7" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H7" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I7" s="25">
+        <v>1</v>
+      </c>
+      <c r="J7" s="25">
+        <v>100</v>
+      </c>
+      <c r="K7" s="25">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="L7" s="25">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="M7" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="N7" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="O7" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P7" s="25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A8" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="31">
         <v>388000</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="31">
         <v>6530000</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="30" t="s">
         <v>2</v>
       </c>
       <c r="E8" s="26">
         <v>20</v>
       </c>
-      <c r="F8" s="27"/>
-      <c r="G8" s="26"/>
-      <c r="I8" s="10"/>
-    </row>
-    <row r="9" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="F8" s="27">
+        <v>2</v>
+      </c>
+      <c r="G8" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H8" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I8" s="25">
+        <v>1</v>
+      </c>
+      <c r="J8" s="25">
+        <v>100</v>
+      </c>
+      <c r="K8" s="25">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="L8" s="25">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="M8" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="N8" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="O8" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P8" s="25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A9" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="31">
         <v>363000</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="31">
         <v>6530000</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="30" t="s">
         <v>2</v>
       </c>
       <c r="E9" s="26">
         <v>5</v>
       </c>
-      <c r="F9" s="27"/>
-      <c r="G9" s="26"/>
-      <c r="I9" s="10"/>
-    </row>
-    <row r="10" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
+      <c r="F9" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="G9" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H9" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I9" s="25">
+        <v>1</v>
+      </c>
+      <c r="J9" s="25">
+        <v>100</v>
+      </c>
+      <c r="K9" s="25">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="L9" s="25">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="M9" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="N9" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="O9" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P9" s="25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A10" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="31">
         <v>372000</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="31">
         <v>6510000</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="30" t="s">
         <v>2</v>
       </c>
       <c r="E10" s="26">
         <v>5</v>
       </c>
-      <c r="F10" s="27"/>
-      <c r="G10" s="26"/>
-      <c r="I10" s="10"/>
-    </row>
-    <row r="11" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
+      <c r="F10" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="G10" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H10" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I10" s="25">
+        <v>1</v>
+      </c>
+      <c r="J10" s="25">
+        <v>100</v>
+      </c>
+      <c r="K10" s="25">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="L10" s="25">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="M10" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="N10" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="O10" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P10" s="25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A11" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="31">
         <v>380000</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="31">
         <v>6535000</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="30" t="s">
         <v>3</v>
       </c>
       <c r="E11" s="26">
         <v>0.1</v>
       </c>
-      <c r="F11" s="27"/>
-      <c r="G11" s="26"/>
-    </row>
-    <row r="12" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
+      <c r="F11" s="27">
+        <v>0.01</v>
+      </c>
+      <c r="G11" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H11" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I11" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="J11" s="25">
+        <v>5</v>
+      </c>
+      <c r="K11" s="25">
+        <f t="shared" si="0"/>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L11" s="25">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="M11" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="N11" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="O11" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P11" s="25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A12" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="31">
         <v>360000</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="31">
         <v>6537000</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="30" t="s">
         <v>3</v>
       </c>
       <c r="E12" s="26">
         <v>0.2</v>
       </c>
-      <c r="F12" s="27"/>
-      <c r="G12" s="26"/>
-    </row>
-    <row r="13" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
+      <c r="F12" s="27">
+        <v>0.02</v>
+      </c>
+      <c r="G12" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H12" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I12" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="J12" s="25">
+        <v>5</v>
+      </c>
+      <c r="K12" s="25">
+        <f t="shared" si="0"/>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L12" s="25">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="M12" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="N12" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="O12" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P12" s="25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A13" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="31">
         <v>370000</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="31">
         <v>6530000</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="30" t="s">
         <v>3</v>
       </c>
       <c r="E13" s="26">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
+      <c r="F13" s="27">
+        <v>0.01</v>
+      </c>
+      <c r="G13" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H13" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I13" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="J13" s="25">
+        <v>5</v>
+      </c>
+      <c r="K13" s="25">
+        <f t="shared" si="0"/>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L13" s="25">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="M13" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="N13" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="O13" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P13" s="25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A14" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="31">
         <v>375000</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="31">
         <v>6520000</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="30" t="s">
         <v>3</v>
       </c>
       <c r="E14" s="26">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
+      <c r="F14" s="27">
+        <v>0.05</v>
+      </c>
+      <c r="G14" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H14" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I14" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="J14" s="25">
+        <v>5</v>
+      </c>
+      <c r="K14" s="25">
+        <f t="shared" si="0"/>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L14" s="25">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="M14" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="N14" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="O14" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P14" s="25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A15" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="31">
         <v>385000</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="31">
         <v>6515000</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="30" t="s">
         <v>3</v>
       </c>
       <c r="E15" s="26">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
+      <c r="F15" s="27">
+        <v>0.03</v>
+      </c>
+      <c r="G15" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H15" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I15" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="J15" s="25">
+        <v>5</v>
+      </c>
+      <c r="K15" s="25">
+        <f t="shared" si="0"/>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L15" s="25">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="M15" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="N15" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="O15" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P15" s="25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A16" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="31">
         <v>375000</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="31">
         <v>6540000</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="30" t="s">
         <v>3</v>
       </c>
       <c r="E16" s="26">
         <v>0.5</v>
       </c>
-      <c r="F16" s="27"/>
-      <c r="G16" s="26"/>
-      <c r="I16" s="10"/>
-    </row>
-    <row r="17" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
+      <c r="F16" s="27">
+        <v>0.05</v>
+      </c>
+      <c r="G16" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H16" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I16" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="J16" s="25">
+        <v>5</v>
+      </c>
+      <c r="K16" s="25">
+        <f t="shared" si="0"/>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L16" s="25">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="M16" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="N16" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="O16" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P16" s="25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A17" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="31">
         <v>388000</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="31">
         <v>6530000</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="30" t="s">
         <v>3</v>
       </c>
       <c r="E17" s="26">
         <v>0.5</v>
       </c>
-      <c r="F17" s="27"/>
-      <c r="G17" s="26"/>
-      <c r="I17" s="10"/>
-    </row>
-    <row r="18" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
+      <c r="F17" s="27">
+        <v>0.05</v>
+      </c>
+      <c r="G17" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H17" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I17" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="J17" s="25">
+        <v>5</v>
+      </c>
+      <c r="K17" s="25">
+        <f t="shared" si="0"/>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L17" s="25">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="M17" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="N17" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="O17" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P17" s="25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A18" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="31">
         <v>363000</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="31">
         <v>6530000</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="30" t="s">
         <v>3</v>
       </c>
       <c r="E18" s="26">
         <v>0.5</v>
       </c>
-      <c r="F18" s="27"/>
-      <c r="G18" s="26"/>
-      <c r="I18" s="10"/>
-    </row>
-    <row r="19" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
+      <c r="F18" s="27">
+        <v>0.05</v>
+      </c>
+      <c r="G18" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H18" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I18" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="J18" s="25">
+        <v>5</v>
+      </c>
+      <c r="K18" s="25">
+        <f t="shared" si="0"/>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L18" s="25">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="M18" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="N18" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="O18" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P18" s="25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A19" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="31">
         <v>372000</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="31">
         <v>6510000</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="30" t="s">
         <v>3</v>
       </c>
       <c r="E19" s="26">
         <v>0.5</v>
       </c>
-      <c r="F19" s="27"/>
-      <c r="G19" s="26"/>
-      <c r="I19" s="10"/>
-    </row>
-    <row r="20" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
+      <c r="F19" s="27">
+        <v>0.05</v>
+      </c>
+      <c r="G19" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H19" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I19" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="J19" s="25">
+        <v>5</v>
+      </c>
+      <c r="K19" s="25">
+        <f t="shared" si="0"/>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L19" s="25">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="M19" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="N19" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="O19" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P19" s="25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A20" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="31">
         <v>380000</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="31">
         <v>6535000</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="30" t="s">
         <v>4</v>
       </c>
       <c r="E20" s="26">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
+      <c r="F20" s="27">
+        <v>0.1</v>
+      </c>
+      <c r="G20" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H20" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I20" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="J20" s="25">
+        <v>10</v>
+      </c>
+      <c r="K20" s="25">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="L20" s="25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M20" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="N20" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="O20" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P20" s="25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A21" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="31">
         <v>360000</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="31">
         <v>6537000</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="30" t="s">
         <v>4</v>
       </c>
       <c r="E21" s="26">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
+      <c r="F21" s="27">
+        <v>0.1</v>
+      </c>
+      <c r="G21" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H21" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I21" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="J21" s="25">
+        <v>10</v>
+      </c>
+      <c r="K21" s="25">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="L21" s="25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M21" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="N21" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="O21" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P21" s="25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A22" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="31">
         <v>370000</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="31">
         <v>6530000</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="30" t="s">
         <v>4</v>
       </c>
       <c r="E22" s="26">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A23" s="19" t="s">
+      <c r="F22" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="G22" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H22" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I22" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="J22" s="25">
+        <v>10</v>
+      </c>
+      <c r="K22" s="25">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="L22" s="25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M22" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="N22" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="O22" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P22" s="25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A23" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="31">
         <v>375000</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="31">
         <v>6520000</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="30" t="s">
         <v>4</v>
       </c>
       <c r="E23" s="26">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A24" s="19" t="s">
+      <c r="F23" s="27">
+        <v>0.1</v>
+      </c>
+      <c r="G23" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H23" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I23" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="J23" s="25">
+        <v>10</v>
+      </c>
+      <c r="K23" s="25">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="L23" s="25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M23" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="N23" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="O23" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P23" s="25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A24" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="31">
         <v>385000</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="31">
         <v>6515000</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D24" s="30" t="s">
         <v>4</v>
       </c>
       <c r="E24" s="26">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A25" s="19" t="s">
+      <c r="F24" s="27">
+        <v>0.05</v>
+      </c>
+      <c r="G24" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H24" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I24" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="J24" s="25">
+        <v>10</v>
+      </c>
+      <c r="K24" s="25">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="L24" s="25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M24" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="N24" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="O24" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P24" s="25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A25" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="31">
         <v>375000</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="31">
         <v>6540000</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D25" s="30" t="s">
         <v>4</v>
       </c>
       <c r="E25" s="26">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A26" s="19" t="s">
+      <c r="F25" s="27">
+        <v>0.1</v>
+      </c>
+      <c r="G25" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H25" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I25" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="J25" s="25">
+        <v>10</v>
+      </c>
+      <c r="K25" s="25">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="L25" s="25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M25" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="N25" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="O25" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P25" s="25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A26" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="31">
         <v>388000</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="31">
         <v>6530000</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D26" s="30" t="s">
         <v>4</v>
       </c>
       <c r="E26" s="26">
         <v>10</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A27" s="19" t="s">
+      <c r="F26" s="27">
+        <v>1</v>
+      </c>
+      <c r="G26" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H26" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I26" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="J26" s="25">
+        <v>10</v>
+      </c>
+      <c r="K26" s="25">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="L26" s="25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M26" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="N26" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="O26" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P26" s="25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A27" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B27" s="31">
         <v>363000</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C27" s="31">
         <v>6530000</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D27" s="30" t="s">
         <v>4</v>
       </c>
       <c r="E27" s="26">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A28" s="19" t="s">
+      <c r="F27" s="27">
+        <v>0.2</v>
+      </c>
+      <c r="G27" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H27" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I27" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="J27" s="25">
+        <v>10</v>
+      </c>
+      <c r="K27" s="25">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="L27" s="25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M27" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="N27" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="O27" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P27" s="25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A28" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B28" s="31">
         <v>372000</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C28" s="31">
         <v>6510000</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="D28" s="30" t="s">
         <v>4</v>
       </c>
       <c r="E28" s="26">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A29" s="19" t="s">
+      <c r="F28" s="27">
+        <v>0.1</v>
+      </c>
+      <c r="G28" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H28" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I28" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="J28" s="25">
+        <v>10</v>
+      </c>
+      <c r="K28" s="25">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="L28" s="25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M28" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="N28" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="O28" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P28" s="25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A29" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B29" s="31">
         <v>380000</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C29" s="31">
         <v>6535000</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D29" s="30" t="s">
         <v>5</v>
       </c>
       <c r="E29" s="26">
         <v>20</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A30" s="19" t="s">
+      <c r="F29" s="27">
+        <v>2</v>
+      </c>
+      <c r="G29" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H29" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I29" s="25">
+        <v>1</v>
+      </c>
+      <c r="J29" s="25">
+        <v>100</v>
+      </c>
+      <c r="K29" s="25">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="L29" s="25">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="M29" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="N29" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="O29" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P29" s="25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A30" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B30" s="31">
         <v>360000</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C30" s="31">
         <v>6537000</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="D30" s="30" t="s">
         <v>5</v>
       </c>
       <c r="E30" s="26">
         <v>40</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A31" s="19" t="s">
+      <c r="F30" s="27">
+        <v>4</v>
+      </c>
+      <c r="G30" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H30" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I30" s="25">
+        <v>1</v>
+      </c>
+      <c r="J30" s="25">
+        <v>100</v>
+      </c>
+      <c r="K30" s="25">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="L30" s="25">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="M30" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="N30" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="O30" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P30" s="25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A31" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="B31" s="5">
+      <c r="B31" s="31">
         <v>370000</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C31" s="31">
         <v>6530000</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="D31" s="30" t="s">
         <v>5</v>
       </c>
       <c r="E31" s="26">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A32" s="19" t="s">
+      <c r="F31" s="27">
+        <v>0.1</v>
+      </c>
+      <c r="G31" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H31" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I31" s="25">
+        <v>1</v>
+      </c>
+      <c r="J31" s="25">
+        <v>100</v>
+      </c>
+      <c r="K31" s="25">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="L31" s="25">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="M31" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="N31" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="O31" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P31" s="25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A32" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="B32" s="5">
+      <c r="B32" s="31">
         <v>375000</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C32" s="31">
         <v>6520000</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="D32" s="30" t="s">
         <v>5</v>
       </c>
       <c r="E32" s="26">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" ht="13" x14ac:dyDescent="0.25">
-      <c r="A33" s="19" t="s">
+      <c r="F32" s="27">
+        <v>3</v>
+      </c>
+      <c r="G32" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H32" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I32" s="25">
+        <v>1</v>
+      </c>
+      <c r="J32" s="25">
+        <v>100</v>
+      </c>
+      <c r="K32" s="25">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="L32" s="25">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="M32" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="N32" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="O32" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P32" s="25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A33" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="B33" s="5">
+      <c r="B33" s="31">
         <v>375000</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C33" s="31">
         <v>6540000</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="D33" s="30" t="s">
         <v>5</v>
       </c>
       <c r="E33" s="26">
         <v>10</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" ht="13" x14ac:dyDescent="0.25">
-      <c r="A34" s="19" t="s">
+      <c r="F33" s="27">
+        <v>1</v>
+      </c>
+      <c r="G33" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H33" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I33" s="25">
+        <v>1</v>
+      </c>
+      <c r="J33" s="25">
+        <v>100</v>
+      </c>
+      <c r="K33" s="25">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="L33" s="25">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="M33" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="N33" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="O33" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P33" s="25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A34" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="B34" s="5">
+      <c r="B34" s="31">
         <v>388000</v>
       </c>
-      <c r="C34" s="5">
+      <c r="C34" s="31">
         <v>6530000</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="D34" s="30" t="s">
         <v>5</v>
       </c>
       <c r="E34" s="26">
         <v>10</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" ht="13" x14ac:dyDescent="0.25">
-      <c r="A35" s="19" t="s">
+      <c r="F34" s="27">
+        <v>1</v>
+      </c>
+      <c r="G34" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H34" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I34" s="25">
+        <v>1</v>
+      </c>
+      <c r="J34" s="25">
+        <v>100</v>
+      </c>
+      <c r="K34" s="25">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="L34" s="25">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="M34" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="N34" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="O34" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P34" s="25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A35" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="B35" s="5">
+      <c r="B35" s="31">
         <v>363000</v>
       </c>
-      <c r="C35" s="5">
+      <c r="C35" s="31">
         <v>6530000</v>
       </c>
-      <c r="D35" s="10" t="s">
+      <c r="D35" s="30" t="s">
         <v>5</v>
       </c>
       <c r="E35" s="26">
         <v>10</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" ht="13" x14ac:dyDescent="0.25">
-      <c r="A36" s="19" t="s">
+      <c r="F35" s="27">
+        <v>1</v>
+      </c>
+      <c r="G35" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H35" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I35" s="25">
+        <v>1</v>
+      </c>
+      <c r="J35" s="25">
+        <v>100</v>
+      </c>
+      <c r="K35" s="25">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="L35" s="25">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="M35" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="N35" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="O35" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P35" s="25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A36" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="B36" s="5">
+      <c r="B36" s="31">
         <v>385000</v>
       </c>
-      <c r="C36" s="5">
+      <c r="C36" s="31">
         <v>6515000</v>
       </c>
-      <c r="D36" s="10" t="s">
+      <c r="D36" s="30" t="s">
         <v>5</v>
       </c>
       <c r="E36" s="26">
         <v>20</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" ht="13" x14ac:dyDescent="0.25">
-      <c r="A37" s="19" t="s">
+      <c r="F36" s="27">
+        <v>2</v>
+      </c>
+      <c r="G36" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H36" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I36" s="25">
+        <v>1</v>
+      </c>
+      <c r="J36" s="25">
+        <v>100</v>
+      </c>
+      <c r="K36" s="25">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="L36" s="25">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="M36" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="N36" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="O36" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P36" s="25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A37" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="B37" s="5">
+      <c r="B37" s="31">
         <v>372000</v>
       </c>
-      <c r="C37" s="5">
+      <c r="C37" s="31">
         <v>6510000</v>
       </c>
-      <c r="D37" s="10" t="s">
+      <c r="D37" s="30" t="s">
         <v>5</v>
       </c>
       <c r="E37" s="26">
         <v>20</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" ht="13" x14ac:dyDescent="0.25">
-      <c r="A38" s="19" t="s">
+      <c r="F37" s="27">
+        <v>2</v>
+      </c>
+      <c r="G37" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H37" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I37" s="25">
+        <v>1</v>
+      </c>
+      <c r="J37" s="25">
+        <v>100</v>
+      </c>
+      <c r="K37" s="25">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="L37" s="25">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="M37" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="N37" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="O37" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P37" s="25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A38" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="B38" s="5">
+      <c r="B38" s="31">
         <v>380000</v>
       </c>
-      <c r="C38" s="5">
+      <c r="C38" s="31">
         <v>6535000</v>
       </c>
-      <c r="D38" s="10" t="s">
+      <c r="D38" s="30" t="s">
         <v>6</v>
       </c>
       <c r="E38" s="26">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" ht="13" x14ac:dyDescent="0.25">
-      <c r="A39" s="19" t="s">
+      <c r="F38" s="27">
+        <v>0.1</v>
+      </c>
+      <c r="G38" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H38" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I38" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="J38" s="25">
+        <v>10</v>
+      </c>
+      <c r="K38" s="25">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="L38" s="25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M38" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="N38" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="O38" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P38" s="25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A39" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="B39" s="5">
+      <c r="B39" s="31">
         <v>360000</v>
       </c>
-      <c r="C39" s="5">
+      <c r="C39" s="31">
         <v>6537000</v>
       </c>
-      <c r="D39" s="10" t="s">
+      <c r="D39" s="30" t="s">
         <v>6</v>
       </c>
       <c r="E39" s="26">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" ht="13" x14ac:dyDescent="0.25">
-      <c r="A40" s="19" t="s">
+      <c r="F39" s="27">
+        <v>0.05</v>
+      </c>
+      <c r="G39" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H39" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I39" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="J39" s="25">
+        <v>10</v>
+      </c>
+      <c r="K39" s="25">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="L39" s="25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M39" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="N39" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="O39" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P39" s="25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A40" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="B40" s="5">
+      <c r="B40" s="31">
         <v>370000</v>
       </c>
-      <c r="C40" s="5">
+      <c r="C40" s="31">
         <v>6530000</v>
       </c>
-      <c r="D40" s="10" t="s">
+      <c r="D40" s="30" t="s">
         <v>6</v>
       </c>
       <c r="E40" s="26">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" ht="13" x14ac:dyDescent="0.25">
-      <c r="A41" s="19" t="s">
+      <c r="F40" s="27">
+        <v>0.02</v>
+      </c>
+      <c r="G40" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H40" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I40" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="J40" s="25">
+        <v>10</v>
+      </c>
+      <c r="K40" s="25">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="L40" s="25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M40" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="N40" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="O40" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P40" s="25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A41" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="B41" s="5">
+      <c r="B41" s="31">
         <v>375000</v>
       </c>
-      <c r="C41" s="5">
+      <c r="C41" s="31">
         <v>6520000</v>
       </c>
-      <c r="D41" s="10" t="s">
+      <c r="D41" s="30" t="s">
         <v>6</v>
       </c>
       <c r="E41" s="26">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" ht="13" x14ac:dyDescent="0.25">
-      <c r="A42" s="19" t="s">
+      <c r="F41" s="27">
+        <v>0.1</v>
+      </c>
+      <c r="G41" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H41" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I41" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="J41" s="25">
+        <v>10</v>
+      </c>
+      <c r="K41" s="25">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="L41" s="25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M41" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="N41" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="O41" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P41" s="25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A42" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="B42" s="5">
+      <c r="B42" s="31">
         <v>385000</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C42" s="31">
         <v>6515000</v>
       </c>
-      <c r="D42" s="10" t="s">
+      <c r="D42" s="30" t="s">
         <v>6</v>
       </c>
       <c r="E42" s="26">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" ht="13" x14ac:dyDescent="0.25">
-      <c r="A43" s="19" t="s">
+      <c r="F42" s="27">
+        <v>0.1</v>
+      </c>
+      <c r="G42" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H42" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I42" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="J42" s="25">
+        <v>10</v>
+      </c>
+      <c r="K42" s="25">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="L42" s="25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M42" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="N42" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="O42" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P42" s="25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A43" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="B43" s="5">
+      <c r="B43" s="31">
         <v>375000</v>
       </c>
-      <c r="C43" s="5">
+      <c r="C43" s="31">
         <v>6540000</v>
       </c>
-      <c r="D43" s="10" t="s">
+      <c r="D43" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E43" s="25">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="13" x14ac:dyDescent="0.25">
-      <c r="A44" s="19" t="s">
+      <c r="E43" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="F43" s="27">
+        <v>0.01</v>
+      </c>
+      <c r="G43" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H43" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I43" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="J43" s="25">
+        <v>10</v>
+      </c>
+      <c r="K43" s="25">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="L43" s="25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M43" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="N43" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="O43" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P43" s="25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A44" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="B44" s="5">
+      <c r="B44" s="31">
         <v>388000</v>
       </c>
-      <c r="C44" s="5">
+      <c r="C44" s="31">
         <v>6530000</v>
       </c>
-      <c r="D44" s="10" t="s">
+      <c r="D44" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E44" s="25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="13" x14ac:dyDescent="0.25">
-      <c r="A45" s="19" t="s">
+      <c r="E44" s="26">
+        <v>1</v>
+      </c>
+      <c r="F44" s="27">
+        <v>0.1</v>
+      </c>
+      <c r="G44" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H44" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I44" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="J44" s="25">
+        <v>10</v>
+      </c>
+      <c r="K44" s="25">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="L44" s="25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M44" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="N44" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="O44" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P44" s="25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A45" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="B45" s="5">
+      <c r="B45" s="31">
         <v>363000</v>
       </c>
-      <c r="C45" s="5">
+      <c r="C45" s="31">
         <v>6530000</v>
       </c>
-      <c r="D45" s="10" t="s">
+      <c r="D45" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E45" s="25">
+      <c r="E45" s="26">
         <v>5</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" ht="13" x14ac:dyDescent="0.25">
-      <c r="A46" s="19" t="s">
+      <c r="F45" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="G45" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H45" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I45" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="J45" s="25">
+        <v>10</v>
+      </c>
+      <c r="K45" s="25">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="L45" s="25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M45" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="N45" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="O45" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P45" s="25">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" ht="12" x14ac:dyDescent="0.3">
+      <c r="A46" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="B46" s="5">
+      <c r="B46" s="31">
         <v>372000</v>
       </c>
-      <c r="C46" s="5">
+      <c r="C46" s="31">
         <v>6510000</v>
       </c>
-      <c r="D46" s="10" t="s">
+      <c r="D46" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E46" s="25">
-        <v>0.1</v>
+      <c r="E46" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="F46" s="27">
+        <v>0.01</v>
+      </c>
+      <c r="G46" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="H46" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I46" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="J46" s="25">
+        <v>10</v>
+      </c>
+      <c r="K46" s="25">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="L46" s="25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M46" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="N46" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="O46" s="25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P46" s="25">
+        <v>1E-4</v>
       </c>
     </row>
   </sheetData>
@@ -2483,4 +4247,1015 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ABC1C0D-065C-43DB-996B-2DB340635848}">
+  <dimension ref="A1:H46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.26953125" style="25" customWidth="1"/>
+    <col min="2" max="2" width="6.26953125" style="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.08984375" style="25" customWidth="1"/>
+    <col min="4" max="4" width="4.54296875" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.453125" style="26" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.36328125" style="26" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.453125" style="26" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.08984375" style="26" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A2" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="37">
+        <v>355120</v>
+      </c>
+      <c r="C2" s="37">
+        <v>6540562</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="48">
+        <v>10</v>
+      </c>
+      <c r="F2" s="49">
+        <v>2</v>
+      </c>
+      <c r="G2" s="48">
+        <v>0.12</v>
+      </c>
+      <c r="H2" s="48">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A3" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="37">
+        <v>364415.7</v>
+      </c>
+      <c r="C3" s="37">
+        <v>6534636</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="48">
+        <v>5</v>
+      </c>
+      <c r="F3" s="49">
+        <v>0.1</v>
+      </c>
+      <c r="G3" s="48">
+        <v>0.2</v>
+      </c>
+      <c r="H3" s="48">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A4" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="37">
+        <v>371000</v>
+      </c>
+      <c r="C4" s="37">
+        <v>6515000</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="48">
+        <v>10</v>
+      </c>
+      <c r="F4" s="49">
+        <v>0.5</v>
+      </c>
+      <c r="G4" s="48">
+        <v>0.08</v>
+      </c>
+      <c r="H4" s="48">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A5" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="37">
+        <v>385447</v>
+      </c>
+      <c r="C5" s="37">
+        <v>6537497</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="48">
+        <v>100</v>
+      </c>
+      <c r="F5" s="49">
+        <v>3</v>
+      </c>
+      <c r="G5" s="48">
+        <v>0.25</v>
+      </c>
+      <c r="H5" s="48">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A6" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="37">
+        <v>385200</v>
+      </c>
+      <c r="C6" s="37">
+        <v>6521000</v>
+      </c>
+      <c r="D6" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="48">
+        <v>10</v>
+      </c>
+      <c r="F6" s="49">
+        <v>0.6</v>
+      </c>
+      <c r="G6" s="48">
+        <v>0.1</v>
+      </c>
+      <c r="H6" s="48">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A7" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="37">
+        <v>372541</v>
+      </c>
+      <c r="C7" s="37">
+        <v>6525478</v>
+      </c>
+      <c r="D7" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="48">
+        <v>2</v>
+      </c>
+      <c r="F7" s="49">
+        <v>0.1</v>
+      </c>
+      <c r="G7" s="48">
+        <v>0.11</v>
+      </c>
+      <c r="H7" s="48">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A8" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="37">
+        <v>367502</v>
+      </c>
+      <c r="C8" s="37">
+        <v>6523500</v>
+      </c>
+      <c r="D8" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="48">
+        <v>20</v>
+      </c>
+      <c r="F8" s="49">
+        <v>2</v>
+      </c>
+      <c r="G8" s="48">
+        <v>0.15</v>
+      </c>
+      <c r="H8" s="48">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A9" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="34">
+        <v>355120</v>
+      </c>
+      <c r="C9" s="34">
+        <v>6540562</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="50">
+        <v>0.1</v>
+      </c>
+      <c r="F9" s="51">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G9" s="50">
+        <v>0.1</v>
+      </c>
+      <c r="H9" s="50">
+        <v>5.0000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A10" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="34">
+        <v>364415.7</v>
+      </c>
+      <c r="C10" s="34">
+        <v>6534636</v>
+      </c>
+      <c r="D10" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="50">
+        <v>0.2</v>
+      </c>
+      <c r="F10" s="51">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G10" s="50">
+        <v>0.1</v>
+      </c>
+      <c r="H10" s="50">
+        <v>6.0000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A11" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="34">
+        <v>371000</v>
+      </c>
+      <c r="C11" s="34">
+        <v>6515000</v>
+      </c>
+      <c r="D11" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="50">
+        <v>0.1</v>
+      </c>
+      <c r="F11" s="51">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G11" s="50">
+        <v>0.1</v>
+      </c>
+      <c r="H11" s="50">
+        <v>9.0000000000000006E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A12" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="34">
+        <v>385447</v>
+      </c>
+      <c r="C12" s="34">
+        <v>6537497</v>
+      </c>
+      <c r="D12" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="50">
+        <v>0.5</v>
+      </c>
+      <c r="F12" s="51">
+        <v>0.05</v>
+      </c>
+      <c r="G12" s="50">
+        <v>0.1</v>
+      </c>
+      <c r="H12" s="50">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A13" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="34">
+        <v>385200</v>
+      </c>
+      <c r="C13" s="34">
+        <v>6521000</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="50">
+        <v>0.3</v>
+      </c>
+      <c r="F13" s="51">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="G13" s="50">
+        <v>0.1</v>
+      </c>
+      <c r="H13" s="50">
+        <v>6.0000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A14" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="34">
+        <v>372541</v>
+      </c>
+      <c r="C14" s="34">
+        <v>6525478</v>
+      </c>
+      <c r="D14" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="50">
+        <v>0.5</v>
+      </c>
+      <c r="F14" s="51">
+        <v>0.04</v>
+      </c>
+      <c r="G14" s="50">
+        <v>0.1</v>
+      </c>
+      <c r="H14" s="50">
+        <v>6.0000000000000002E-6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A15" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="34">
+        <v>367502</v>
+      </c>
+      <c r="C15" s="34">
+        <v>6523500</v>
+      </c>
+      <c r="D15" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="50">
+        <v>0.5</v>
+      </c>
+      <c r="F15" s="51">
+        <v>0.01</v>
+      </c>
+      <c r="G15" s="50">
+        <v>0.1</v>
+      </c>
+      <c r="H15" s="50">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A16" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="40">
+        <v>355120</v>
+      </c>
+      <c r="C16" s="40">
+        <v>6540562</v>
+      </c>
+      <c r="D16" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="52">
+        <v>1</v>
+      </c>
+      <c r="F16" s="53">
+        <v>0.02</v>
+      </c>
+      <c r="G16" s="52">
+        <v>0.1</v>
+      </c>
+      <c r="H16" s="52">
+        <v>4.0000000000000003E-5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A17" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="40">
+        <v>364415.7</v>
+      </c>
+      <c r="C17" s="40">
+        <v>6534636</v>
+      </c>
+      <c r="D17" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="52">
+        <v>1</v>
+      </c>
+      <c r="F17" s="53">
+        <v>0.2</v>
+      </c>
+      <c r="G17" s="52">
+        <v>0.1</v>
+      </c>
+      <c r="H17" s="52">
+        <v>9.0000000000000006E-5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A18" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="40">
+        <v>371000</v>
+      </c>
+      <c r="C18" s="40">
+        <v>6515000</v>
+      </c>
+      <c r="D18" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="52">
+        <v>5</v>
+      </c>
+      <c r="F18" s="53">
+        <v>0.7</v>
+      </c>
+      <c r="G18" s="52">
+        <v>0.1</v>
+      </c>
+      <c r="H18" s="52">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A19" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="40">
+        <v>385447</v>
+      </c>
+      <c r="C19" s="40">
+        <v>6537497</v>
+      </c>
+      <c r="D19" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" s="52">
+        <v>1</v>
+      </c>
+      <c r="F19" s="53">
+        <v>0.05</v>
+      </c>
+      <c r="G19" s="52">
+        <v>0.1</v>
+      </c>
+      <c r="H19" s="52">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A20" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="40">
+        <v>385200</v>
+      </c>
+      <c r="C20" s="40">
+        <v>6521000</v>
+      </c>
+      <c r="D20" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="52">
+        <v>0.5</v>
+      </c>
+      <c r="F20" s="53">
+        <v>0.2</v>
+      </c>
+      <c r="G20" s="52">
+        <v>0.1</v>
+      </c>
+      <c r="H20" s="52">
+        <v>6.0000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A21" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="40">
+        <v>372541</v>
+      </c>
+      <c r="C21" s="40">
+        <v>6525478</v>
+      </c>
+      <c r="D21" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" s="52">
+        <v>1</v>
+      </c>
+      <c r="F21" s="53">
+        <v>0.2</v>
+      </c>
+      <c r="G21" s="52">
+        <v>0.1</v>
+      </c>
+      <c r="H21" s="52">
+        <v>4.0000000000000003E-5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A22" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="40">
+        <v>367502</v>
+      </c>
+      <c r="C22" s="40">
+        <v>6523500</v>
+      </c>
+      <c r="D22" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" s="52">
+        <v>10</v>
+      </c>
+      <c r="F22" s="53">
+        <v>0.5</v>
+      </c>
+      <c r="G22" s="52">
+        <v>0.1</v>
+      </c>
+      <c r="H22" s="52">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A23" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="43">
+        <v>355120</v>
+      </c>
+      <c r="C23" s="43">
+        <v>6540562</v>
+      </c>
+      <c r="D23" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" s="54">
+        <v>2</v>
+      </c>
+      <c r="F23" s="55">
+        <v>0.5</v>
+      </c>
+      <c r="G23" s="54">
+        <v>0.1</v>
+      </c>
+      <c r="H23" s="54">
+        <v>3.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A24" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="43">
+        <v>364415.7</v>
+      </c>
+      <c r="C24" s="43">
+        <v>6534636</v>
+      </c>
+      <c r="D24" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" s="54">
+        <v>40</v>
+      </c>
+      <c r="F24" s="55">
+        <v>1</v>
+      </c>
+      <c r="G24" s="54">
+        <v>0.1</v>
+      </c>
+      <c r="H24" s="54">
+        <v>9.0000000000000006E-5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A25" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="43">
+        <v>371000</v>
+      </c>
+      <c r="C25" s="43">
+        <v>6515000</v>
+      </c>
+      <c r="D25" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="54">
+        <v>1</v>
+      </c>
+      <c r="F25" s="55">
+        <v>1</v>
+      </c>
+      <c r="G25" s="54">
+        <v>0.1</v>
+      </c>
+      <c r="H25" s="54">
+        <v>8.9999999999999998E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A26" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="43">
+        <v>385447</v>
+      </c>
+      <c r="C26" s="43">
+        <v>6537497</v>
+      </c>
+      <c r="D26" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" s="54">
+        <v>30</v>
+      </c>
+      <c r="F26" s="55">
+        <v>1</v>
+      </c>
+      <c r="G26" s="54">
+        <v>0.1</v>
+      </c>
+      <c r="H26" s="54">
+        <v>6.9999999999999994E-5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A27" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="43">
+        <v>385200</v>
+      </c>
+      <c r="C27" s="43">
+        <v>6521000</v>
+      </c>
+      <c r="D27" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="54">
+        <v>10</v>
+      </c>
+      <c r="F27" s="55">
+        <v>0.06</v>
+      </c>
+      <c r="G27" s="54">
+        <v>0.1</v>
+      </c>
+      <c r="H27" s="54">
+        <v>6.0000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A28" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="43">
+        <v>372541</v>
+      </c>
+      <c r="C28" s="43">
+        <v>6525478</v>
+      </c>
+      <c r="D28" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="54">
+        <v>10</v>
+      </c>
+      <c r="F28" s="55">
+        <v>1</v>
+      </c>
+      <c r="G28" s="54">
+        <v>0.1</v>
+      </c>
+      <c r="H28" s="54">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A29" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="43">
+        <v>367502</v>
+      </c>
+      <c r="C29" s="43">
+        <v>6523500</v>
+      </c>
+      <c r="D29" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29" s="54">
+        <v>20</v>
+      </c>
+      <c r="F29" s="55">
+        <v>0.5</v>
+      </c>
+      <c r="G29" s="54">
+        <v>0.1</v>
+      </c>
+      <c r="H29" s="54">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A30" s="45" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="46">
+        <v>355120</v>
+      </c>
+      <c r="C30" s="46">
+        <v>6540562</v>
+      </c>
+      <c r="D30" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="56">
+        <v>1</v>
+      </c>
+      <c r="F30" s="57">
+        <v>0.05</v>
+      </c>
+      <c r="G30" s="56">
+        <v>0.1</v>
+      </c>
+      <c r="H30" s="56">
+        <v>2.0000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A31" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" s="46">
+        <v>364415.7</v>
+      </c>
+      <c r="C31" s="46">
+        <v>6534636</v>
+      </c>
+      <c r="D31" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="56">
+        <v>0.5</v>
+      </c>
+      <c r="F31" s="57">
+        <v>0.2</v>
+      </c>
+      <c r="G31" s="56">
+        <v>0.1</v>
+      </c>
+      <c r="H31" s="56">
+        <v>6.9999999999999994E-5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A32" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32" s="46">
+        <v>371000</v>
+      </c>
+      <c r="C32" s="46">
+        <v>6515000</v>
+      </c>
+      <c r="D32" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" s="56">
+        <v>0.2</v>
+      </c>
+      <c r="F32" s="57">
+        <v>0.1</v>
+      </c>
+      <c r="G32" s="56">
+        <v>0.1</v>
+      </c>
+      <c r="H32" s="56">
+        <v>9.0000000000000006E-5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A33" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="46">
+        <v>385447</v>
+      </c>
+      <c r="C33" s="46">
+        <v>6537497</v>
+      </c>
+      <c r="D33" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="56">
+        <v>1</v>
+      </c>
+      <c r="F33" s="57">
+        <v>0.01</v>
+      </c>
+      <c r="G33" s="56">
+        <v>0.1</v>
+      </c>
+      <c r="H33" s="56">
+        <v>8.9999999999999998E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A34" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="46">
+        <v>385200</v>
+      </c>
+      <c r="C34" s="46">
+        <v>6521000</v>
+      </c>
+      <c r="D34" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" s="56">
+        <v>1</v>
+      </c>
+      <c r="F34" s="57">
+        <v>0.02</v>
+      </c>
+      <c r="G34" s="56">
+        <v>0.1</v>
+      </c>
+      <c r="H34" s="56">
+        <v>3.0000000000000001E-6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A35" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35" s="46">
+        <v>372541</v>
+      </c>
+      <c r="C35" s="46">
+        <v>6525478</v>
+      </c>
+      <c r="D35" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" s="56">
+        <v>0.1</v>
+      </c>
+      <c r="F35" s="57">
+        <v>0.1</v>
+      </c>
+      <c r="G35" s="56">
+        <v>0.1</v>
+      </c>
+      <c r="H35" s="56">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A36" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="B36" s="46">
+        <v>367502</v>
+      </c>
+      <c r="C36" s="46">
+        <v>6523500</v>
+      </c>
+      <c r="D36" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" s="56">
+        <v>1</v>
+      </c>
+      <c r="F36" s="57">
+        <v>0.5</v>
+      </c>
+      <c r="G36" s="56">
+        <v>0.1</v>
+      </c>
+      <c r="H36" s="56">
+        <v>4.0000000000000003E-5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A37" s="32"/>
+      <c r="B37" s="31"/>
+      <c r="C37" s="31"/>
+    </row>
+    <row r="38" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A38" s="32"/>
+      <c r="B38" s="31"/>
+      <c r="C38" s="31"/>
+    </row>
+    <row r="39" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A39" s="32"/>
+      <c r="B39" s="31"/>
+      <c r="C39" s="31"/>
+    </row>
+    <row r="40" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A40" s="32"/>
+      <c r="B40" s="31"/>
+      <c r="C40" s="31"/>
+    </row>
+    <row r="41" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A41" s="32"/>
+      <c r="B41" s="31"/>
+      <c r="C41" s="31"/>
+    </row>
+    <row r="42" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A42" s="32"/>
+      <c r="B42" s="31"/>
+      <c r="C42" s="31"/>
+    </row>
+    <row r="43" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A43" s="32"/>
+      <c r="B43" s="31"/>
+      <c r="C43" s="31"/>
+    </row>
+    <row r="44" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A44" s="32"/>
+      <c r="B44" s="31"/>
+      <c r="C44" s="31"/>
+    </row>
+    <row r="45" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A45" s="32"/>
+      <c r="B45" s="31"/>
+      <c r="C45" s="31"/>
+    </row>
+    <row r="46" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+      <c r="A46" s="32"/>
+      <c r="B46" s="31"/>
+      <c r="C46" s="31"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>